<commit_message>
[WIP] Add default_code column, update matching to default_code Update column order Update tests Update formatting of cells
</commit_message>
<xml_diff>
--- a/stock_orderpoint_impex_matrix/tests/fixtures/bad_structure.xlsx
+++ b/stock_orderpoint_impex_matrix/tests/fixtures/bad_structure.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t xml:space="preserve">Entrepôt YourCompany</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">Entrepôt Demo OP WH</t>
   </si>
   <si>
+    <t xml:space="preserve">Code Article</t>
+  </si>
+  <si>
     <t xml:space="preserve">Article</t>
   </si>
   <si>
@@ -47,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">Extra column here</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-COM11</t>
   </si>
   <si>
     <t xml:space="preserve">Cabinet with Doors</t>
@@ -125,8 +131,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -147,29 +157,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V2" activeCellId="0" sqref="M:V"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="6" min="5" style="0" width="13.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="11" min="10" style="0" width="24.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="24.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="7" min="6" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="24.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="12" min="11" style="0" width="24.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="24.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>1</v>
       </c>
     </row>
@@ -193,7 +203,7 @@
         <v>7</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>4</v>
@@ -210,39 +220,45 @@
       <c r="L2" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="M2" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="0" t="n">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="D3" s="0" t="n">
         <v>5.55</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="E3" s="0" t="n">
         <v>6.66</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="F3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="I3" s="0" t="n">
         <v>11.11</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="J3" s="0" t="n">
         <v>12.12</v>
       </c>
-      <c r="J3" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="K3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="0" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>